<commit_message>
mas canales a base de datos
</commit_message>
<xml_diff>
--- a/cypher.xlsx
+++ b/cypher.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LUIS PEDRO\Proyecto2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/81d0a113b1b3462a/Estructura de datos/Proyecto2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6435BB62-6019-47CE-9981-6558E1FAF786}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{6435BB62-6019-47CE-9981-6558E1FAF786}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A3F5B76A-8E94-4CF7-91C1-6129CE8AC320}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5B033F08-1B63-401B-9668-7FAFF3FA6715}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="NOdos" sheetId="2" r:id="rId1"/>
     <sheet name="Hoja1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="243">
   <si>
     <t>Creating nodes</t>
   </si>
@@ -698,6 +700,69 @@
   </si>
   <si>
     <t>https://www.youtube.com/channel/UCzmN6x2tl-OaQPvUwesoh4w</t>
+  </si>
+  <si>
+    <t>n28</t>
+  </si>
+  <si>
+    <t>Chloe Ting</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/channel/UCCgLoMYIyP0U56dEhEL1wXQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Activo </t>
+  </si>
+  <si>
+    <t>n29</t>
+  </si>
+  <si>
+    <t>MadFit</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/channel/UCpQ34afVgk8cRQBjSJ1xuJQ</t>
+  </si>
+  <si>
+    <t>n30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POPSUGAR fitness </t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/channel/UCBINFWq52ShSgUFEoynfSwg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cardio </t>
+  </si>
+  <si>
+    <t>n31</t>
+  </si>
+  <si>
+    <t>Pamela Reif</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/channel/UChVRfsT_ASBZk10o0An7Ucg</t>
+  </si>
+  <si>
+    <t>n32</t>
+  </si>
+  <si>
+    <t>Calisthenicmovement</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/channel/UCZIIRX8rkNjVpP-oLMHpeDw</t>
+  </si>
+  <si>
+    <t>n33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stretching </t>
+  </si>
+  <si>
+    <t>ACTIV CHIROPRACTIC</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/channel/UCoQfmeUjWSAN6bJ73p8yriA</t>
   </si>
 </sst>
 </file>
@@ -1178,7 +1243,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1309,7 +1374,7 @@
         <v>15</v>
       </c>
       <c r="H5" t="str">
-        <f t="shared" ref="H5:H29" si="0">"CREATE("&amp;A5&amp;":canal{name:'"&amp;B5&amp;"',link:'"&amp;C5&amp;"',duracion:'"&amp;D5&amp;"',esDinamico:'"&amp;E5&amp;"',es_ejercicio:'"&amp;F5&amp;"',tipoVideo:'"&amp;G5&amp;"'})"</f>
+        <f t="shared" ref="H5:H35" si="0">"CREATE("&amp;A5&amp;":canal{name:'"&amp;B5&amp;"',link:'"&amp;C5&amp;"',duracion:'"&amp;D5&amp;"',esDinamico:'"&amp;E5&amp;"',es_ejercicio:'"&amp;F5&amp;"',tipoVideo:'"&amp;G5&amp;"'})"</f>
         <v>CREATE(n3:canal{name:'Xuan Lan Yoga',link:'https://www.youtube.com/user/yogalanbcn',duracion:'45 min promedio',esDinamico:'Pasivo',es_ejercicio:'Yoga',tipoVideo:'En Vivo'})</v>
       </c>
     </row>
@@ -1962,60 +2027,168 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
+      <c r="A30" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="G30" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H30" t="str">
+        <f t="shared" si="0"/>
+        <v>CREATE(n28:canal{name:'Chloe Ting',link:'https://www.youtube.com/channel/UCCgLoMYIyP0U56dEhEL1wXQ',duracion:'15 min promedio',esDinamico:'Activo ',es_ejercicio:'Body Building',tipoVideo:'Pre Grabadas'})</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
+      <c r="A31" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H31" t="str">
+        <f t="shared" si="0"/>
+        <v>CREATE(n29:canal{name:'MadFit',link:'https://www.youtube.com/channel/UCpQ34afVgk8cRQBjSJ1xuJQ',duracion:'20 min promedio',esDinamico:'Activo',es_ejercicio:'Pilates',tipoVideo:'Pre Grabadas'})</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
-      <c r="B35" s="9"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="G32" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H32" t="str">
+        <f t="shared" si="0"/>
+        <v>CREATE(n30:canal{name:'POPSUGAR fitness ',link:'https://www.youtube.com/channel/UCBINFWq52ShSgUFEoynfSwg',duracion:'30 min promedio',esDinamico:'Activo',es_ejercicio:'Cardio ',tipoVideo:'Pre Grabadas'})</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="G33" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H33" t="str">
+        <f t="shared" si="0"/>
+        <v>CREATE(n31:canal{name:'Pamela Reif',link:'https://www.youtube.com/channel/UChVRfsT_ASBZk10o0An7Ucg',duracion:'30 min promedio',esDinamico:'Activo',es_ejercicio:'Body Building',tipoVideo:'En Vivo'})</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G34" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H34" t="str">
+        <f t="shared" si="0"/>
+        <v>CREATE(n32:canal{name:'Calisthenicmovement',link:'https://www.youtube.com/channel/UCZIIRX8rkNjVpP-oLMHpeDw',duracion:'10 min promedio',esDinamico:'Activo',es_ejercicio:'Calistenia',tipoVideo:'Pre Grabadas'})</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="G35" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H35" t="str">
+        <f t="shared" si="0"/>
+        <v>CREATE(n33:canal{name:'ACTIV CHIROPRACTIC',link:'https://www.youtube.com/channel/UCoQfmeUjWSAN6bJ73p8yriA',duracion:'10 min promedio',esDinamico:'Pasivo',es_ejercicio:'Stretching ',tipoVideo:'Pre Grabadas'})</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="9"/>
       <c r="C36" s="2"/>
@@ -2024,7 +2197,7 @@
       <c r="F36" s="12"/>
       <c r="G36" s="12"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="9"/>
       <c r="C37" s="2"/>
@@ -2033,7 +2206,7 @@
       <c r="F37" s="12"/>
       <c r="G37" s="12"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="9"/>
       <c r="C38" s="2"/>
@@ -2075,9 +2248,15 @@
     <hyperlink ref="C27" r:id="rId25" xr:uid="{68EF3D18-C6CA-40D1-AE3A-9E3C2334263F}"/>
     <hyperlink ref="C28" r:id="rId26" xr:uid="{AAEFB9B9-2C71-4342-AEB0-0FF7AFE3793C}"/>
     <hyperlink ref="C29" r:id="rId27" xr:uid="{C31D0B92-A5C4-40DB-9E69-AAA9231F79FF}"/>
+    <hyperlink ref="C30" r:id="rId28" xr:uid="{089631AC-9A2E-40E4-8E1B-134F375BCDFE}"/>
+    <hyperlink ref="C31" r:id="rId29" xr:uid="{4F730B0A-5097-467A-9A11-F20496C7305A}"/>
+    <hyperlink ref="C32" r:id="rId30" xr:uid="{1961E62E-C78E-4950-8DAD-AFB140BD6655}"/>
+    <hyperlink ref="C33" r:id="rId31" xr:uid="{D32C7F0B-B844-452E-8F52-19EFB89D140F}"/>
+    <hyperlink ref="C34" r:id="rId32" xr:uid="{ABC76B22-9F61-47DA-9CE0-E1D88379A802}"/>
+    <hyperlink ref="C35" r:id="rId33" xr:uid="{82A00083-CFD9-4A7F-8553-9845489A0BE3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId28"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId34"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
cambios a base de datos
</commit_message>
<xml_diff>
--- a/cypher.xlsx
+++ b/cypher.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/81d0a113b1b3462a/Estructura de datos/Proyecto2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maris\Proyecto2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{6435BB62-6019-47CE-9981-6558E1FAF786}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A3F5B76A-8E94-4CF7-91C1-6129CE8AC320}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D21DA9C-0589-4BE7-91DE-F0A1082FA8C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5B033F08-1B63-401B-9668-7FAFF3FA6715}"/>
+    <workbookView xWindow="300" yWindow="210" windowWidth="20190" windowHeight="11310" xr2:uid="{5B033F08-1B63-401B-9668-7FAFF3FA6715}"/>
   </bookViews>
   <sheets>
     <sheet name="NOdos" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="239">
   <si>
     <t>Creating nodes</t>
   </si>
@@ -645,27 +645,18 @@
     <t>https://www.youtube.com/user/icecream4PRs</t>
   </si>
   <si>
-    <t xml:space="preserve"> 10 min promedio</t>
-  </si>
-  <si>
     <t>ATHLEAN-X</t>
   </si>
   <si>
     <t>https://www.youtube.com/channel/UCe0TLA0EsQbE-MjuHXevj2A</t>
   </si>
   <si>
-    <t>8 min promedio</t>
-  </si>
-  <si>
     <t>SarahBethYoga</t>
   </si>
   <si>
     <t>https://www.youtube.com/user/SarahBethShow</t>
   </si>
   <si>
-    <t>20 min promedio</t>
-  </si>
-  <si>
     <t>BrettLarkinYoga</t>
   </si>
   <si>
@@ -688,9 +679,6 @@
   </si>
   <si>
     <t>https://www.youtube.com/user/TheMiamiTrainer</t>
-  </si>
-  <si>
-    <t>10 min promedio</t>
   </si>
   <si>
     <t>n27</t>
@@ -922,7 +910,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -944,7 +932,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1242,11 +1230,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24E2E661-1920-4F02-ABE9-5F6ACBCBD314}">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.42578125" customWidth="1"/>
     <col min="3" max="3" width="69.7109375" bestFit="1" customWidth="1"/>
@@ -1794,7 +1782,7 @@
         <v>200</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>203</v>
+        <v>9</v>
       </c>
       <c r="E21" s="13" t="s">
         <v>136</v>
@@ -1807,7 +1795,7 @@
       </c>
       <c r="H21" t="str">
         <f t="shared" si="0"/>
-        <v>CREATE(n19:canal{name:'Jeremy Ethier',link:'https://www.youtube.com/channel/UCERm5yFZ1SptUEU4wZ2vJvw',duracion:' 10 min promedio',esDinamico:'Pasivo',es_ejercicio:'Body Building',tipoVideo:'Pre Grabadas'})</v>
+        <v>CREATE(n19:canal{name:'Jeremy Ethier',link:'https://www.youtube.com/channel/UCERm5yFZ1SptUEU4wZ2vJvw',duracion:'menos 15 min',esDinamico:'Pasivo',es_ejercicio:'Body Building',tipoVideo:'Pre Grabadas'})</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1842,13 +1830,13 @@
         <v>193</v>
       </c>
       <c r="B23" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="C23" s="15" t="s">
         <v>204</v>
       </c>
-      <c r="C23" s="15" t="s">
-        <v>205</v>
-      </c>
       <c r="D23" s="13" t="s">
-        <v>206</v>
+        <v>9</v>
       </c>
       <c r="E23" s="13" t="s">
         <v>136</v>
@@ -1861,7 +1849,7 @@
       </c>
       <c r="H23" t="str">
         <f t="shared" si="0"/>
-        <v>CREATE(n21:canal{name:'ATHLEAN-X',link:'https://www.youtube.com/channel/UCe0TLA0EsQbE-MjuHXevj2A',duracion:'8 min promedio',esDinamico:'Pasivo',es_ejercicio:'Body Building',tipoVideo:'Pre Grabadas'})</v>
+        <v>CREATE(n21:canal{name:'ATHLEAN-X',link:'https://www.youtube.com/channel/UCe0TLA0EsQbE-MjuHXevj2A',duracion:'menos 15 min',esDinamico:'Pasivo',es_ejercicio:'Body Building',tipoVideo:'Pre Grabadas'})</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1869,13 +1857,13 @@
         <v>194</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>209</v>
+        <v>11</v>
       </c>
       <c r="E24" s="13" t="s">
         <v>7</v>
@@ -1888,7 +1876,7 @@
       </c>
       <c r="H24" t="str">
         <f t="shared" si="0"/>
-        <v>CREATE(n22:canal{name:'SarahBethYoga',link:'https://www.youtube.com/user/SarahBethShow',duracion:'20 min promedio',esDinamico:'Activo',es_ejercicio:'Yoga',tipoVideo:'Pre Grabadas'})</v>
+        <v>CREATE(n22:canal{name:'SarahBethYoga',link:'https://www.youtube.com/user/SarahBethShow',duracion:'30 min promedio',esDinamico:'Activo',es_ejercicio:'Yoga',tipoVideo:'Pre Grabadas'})</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1896,10 +1884,10 @@
         <v>195</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D25" s="13" t="s">
         <v>10</v>
@@ -1923,10 +1911,10 @@
         <v>196</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D26" s="13" t="s">
         <v>10</v>
@@ -1950,13 +1938,13 @@
         <v>197</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>206</v>
+        <v>9</v>
       </c>
       <c r="E27" s="13" t="s">
         <v>7</v>
@@ -1969,7 +1957,7 @@
       </c>
       <c r="H27" t="str">
         <f t="shared" si="0"/>
-        <v>CREATE(n25:canal{name:'Austin Dunham',link:'https://www.youtube.com/user/GeekAMD',duracion:'8 min promedio',esDinamico:'Activo',es_ejercicio:'Calistenia',tipoVideo:'Pre Grabadas'})</v>
+        <v>CREATE(n25:canal{name:'Austin Dunham',link:'https://www.youtube.com/user/GeekAMD',duracion:'menos 15 min',esDinamico:'Activo',es_ejercicio:'Calistenia',tipoVideo:'Pre Grabadas'})</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1977,13 +1965,13 @@
         <v>198</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>218</v>
+        <v>9</v>
       </c>
       <c r="E28" s="13" t="s">
         <v>7</v>
@@ -1996,21 +1984,21 @@
       </c>
       <c r="H28" t="str">
         <f t="shared" si="0"/>
-        <v>CREATE(n26:canal{name:'OFFICIALTHENX',link:'https://www.youtube.com/user/TheMiamiTrainer',duracion:'10 min promedio',esDinamico:'Activo',es_ejercicio:'Calistenia',tipoVideo:'Pre Grabadas'})</v>
+        <v>CREATE(n26:canal{name:'OFFICIALTHENX',link:'https://www.youtube.com/user/TheMiamiTrainer',duracion:'menos 15 min',esDinamico:'Activo',es_ejercicio:'Calistenia',tipoVideo:'Pre Grabadas'})</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>206</v>
+        <v>9</v>
       </c>
       <c r="E29" s="13" t="s">
         <v>7</v>
@@ -2023,24 +2011,24 @@
       </c>
       <c r="H29" t="str">
         <f t="shared" si="0"/>
-        <v>CREATE(n27:canal{name:'Osvaldo Lugones',link:'https://www.youtube.com/channel/UCzmN6x2tl-OaQPvUwesoh4w',duracion:'8 min promedio',esDinamico:'Activo',es_ejercicio:'Calistenia',tipoVideo:'Pre Grabadas'})</v>
+        <v>CREATE(n27:canal{name:'Osvaldo Lugones',link:'https://www.youtube.com/channel/UCzmN6x2tl-OaQPvUwesoh4w',duracion:'menos 15 min',esDinamico:'Activo',es_ejercicio:'Calistenia',tipoVideo:'Pre Grabadas'})</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D30" s="13" t="s">
         <v>10</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="F30" s="13" t="s">
         <v>22</v>
@@ -2055,16 +2043,16 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>209</v>
+        <v>11</v>
       </c>
       <c r="E31" s="13" t="s">
         <v>7</v>
@@ -2077,18 +2065,18 @@
       </c>
       <c r="H31" t="str">
         <f t="shared" si="0"/>
-        <v>CREATE(n29:canal{name:'MadFit',link:'https://www.youtube.com/channel/UCpQ34afVgk8cRQBjSJ1xuJQ',duracion:'20 min promedio',esDinamico:'Activo',es_ejercicio:'Pilates',tipoVideo:'Pre Grabadas'})</v>
+        <v>CREATE(n29:canal{name:'MadFit',link:'https://www.youtube.com/channel/UCpQ34afVgk8cRQBjSJ1xuJQ',duracion:'30 min promedio',esDinamico:'Activo',es_ejercicio:'Pilates',tipoVideo:'Pre Grabadas'})</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="D32" s="13" t="s">
         <v>11</v>
@@ -2097,7 +2085,7 @@
         <v>7</v>
       </c>
       <c r="F32" s="13" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="G32" s="13" t="s">
         <v>16</v>
@@ -2109,13 +2097,13 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D33" s="13" t="s">
         <v>11</v>
@@ -2136,16 +2124,16 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>218</v>
+        <v>9</v>
       </c>
       <c r="E34" s="13" t="s">
         <v>7</v>
@@ -2158,34 +2146,34 @@
       </c>
       <c r="H34" t="str">
         <f t="shared" si="0"/>
-        <v>CREATE(n32:canal{name:'Calisthenicmovement',link:'https://www.youtube.com/channel/UCZIIRX8rkNjVpP-oLMHpeDw',duracion:'10 min promedio',esDinamico:'Activo',es_ejercicio:'Calistenia',tipoVideo:'Pre Grabadas'})</v>
+        <v>CREATE(n32:canal{name:'Calisthenicmovement',link:'https://www.youtube.com/channel/UCZIIRX8rkNjVpP-oLMHpeDw',duracion:'menos 15 min',esDinamico:'Activo',es_ejercicio:'Calistenia',tipoVideo:'Pre Grabadas'})</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>218</v>
+        <v>9</v>
       </c>
       <c r="E35" s="13" t="s">
         <v>136</v>
       </c>
       <c r="F35" s="13" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="G35" s="13" t="s">
         <v>16</v>
       </c>
       <c r="H35" t="str">
         <f t="shared" si="0"/>
-        <v>CREATE(n33:canal{name:'ACTIV CHIROPRACTIC',link:'https://www.youtube.com/channel/UCoQfmeUjWSAN6bJ73p8yriA',duracion:'10 min promedio',esDinamico:'Pasivo',es_ejercicio:'Stretching ',tipoVideo:'Pre Grabadas'})</v>
+        <v>CREATE(n33:canal{name:'ACTIV CHIROPRACTIC',link:'https://www.youtube.com/channel/UCoQfmeUjWSAN6bJ73p8yriA',duracion:'menos 15 min',esDinamico:'Pasivo',es_ejercicio:'Stretching ',tipoVideo:'Pre Grabadas'})</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -2268,7 +2256,7 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="69.7109375" bestFit="1" customWidth="1"/>

</xml_diff>